<commit_message>
finished all functions in "All Roles" section and fixed some bugs in general.cpp
Also updated my progress in the excel file
</commit_message>
<xml_diff>
--- a/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
+++ b/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D90A3D2-1E66-4412-9F90-5608D8C4A77F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A813B4-AD2C-4976-9F6F-5F2AB91378B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2104,11 +2104,11 @@
   <dimension ref="A1:BO81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="K34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="6" topLeftCell="AB10" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomRight" activeCell="AI16" sqref="AI16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2723,7 +2723,9 @@
       <c r="G10" s="14">
         <v>13</v>
       </c>
-      <c r="H10" s="14"/>
+      <c r="H10" s="14">
+        <v>2</v>
+      </c>
       <c r="I10" s="15">
         <v>1</v>
       </c>
@@ -2743,9 +2745,15 @@
       <c r="F11" s="14">
         <v>4</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="15"/>
+      <c r="G11" s="14">
+        <v>15</v>
+      </c>
+      <c r="H11" s="14">
+        <v>1</v>
+      </c>
+      <c r="I11" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="47">
@@ -2787,9 +2795,15 @@
       <c r="F13" s="14">
         <v>4</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="15"/>
+      <c r="G13" s="14">
+        <v>15</v>
+      </c>
+      <c r="H13" s="14">
+        <v>1</v>
+      </c>
+      <c r="I13" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="46">
@@ -2946,8 +2960,12 @@
       </c>
       <c r="C23" s="28"/>
       <c r="D23" s="29"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
+      <c r="E23" s="14">
+        <v>19</v>
+      </c>
+      <c r="F23" s="14">
+        <v>14</v>
+      </c>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="15"/>
@@ -2961,8 +2979,12 @@
       </c>
       <c r="C24" s="28"/>
       <c r="D24" s="29"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
+      <c r="E24" s="14">
+        <v>19</v>
+      </c>
+      <c r="F24" s="14">
+        <v>14</v>
+      </c>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="15"/>
@@ -2976,8 +2998,12 @@
       </c>
       <c r="C25" s="28"/>
       <c r="D25" s="29"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
+      <c r="E25" s="14">
+        <v>19</v>
+      </c>
+      <c r="F25" s="14">
+        <v>14</v>
+      </c>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
       <c r="I25" s="15"/>
@@ -2991,8 +3017,12 @@
       </c>
       <c r="C26" s="28"/>
       <c r="D26" s="29"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
+      <c r="E26" s="14">
+        <v>19</v>
+      </c>
+      <c r="F26" s="14">
+        <v>14</v>
+      </c>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
       <c r="I26" s="15"/>
@@ -3006,8 +3036,12 @@
       </c>
       <c r="C27" s="28"/>
       <c r="D27" s="29"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
+      <c r="E27" s="14">
+        <v>19</v>
+      </c>
+      <c r="F27" s="14">
+        <v>14</v>
+      </c>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
       <c r="I27" s="15"/>
@@ -3021,8 +3055,12 @@
       </c>
       <c r="C28" s="28"/>
       <c r="D28" s="29"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
+      <c r="E28" s="14">
+        <v>19</v>
+      </c>
+      <c r="F28" s="14">
+        <v>14</v>
+      </c>
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
       <c r="I28" s="15"/>
@@ -3036,8 +3074,12 @@
       </c>
       <c r="C29" s="28"/>
       <c r="D29" s="29"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
+      <c r="E29" s="14">
+        <v>19</v>
+      </c>
+      <c r="F29" s="14">
+        <v>14</v>
+      </c>
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
       <c r="I29" s="15"/>
@@ -3051,8 +3093,12 @@
       </c>
       <c r="C30" s="28"/>
       <c r="D30" s="29"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
+      <c r="E30" s="14">
+        <v>19</v>
+      </c>
+      <c r="F30" s="14">
+        <v>14</v>
+      </c>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
       <c r="I30" s="15"/>
@@ -3066,8 +3112,12 @@
       </c>
       <c r="C31" s="28"/>
       <c r="D31" s="29"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
+      <c r="E31" s="14">
+        <v>19</v>
+      </c>
+      <c r="F31" s="14">
+        <v>14</v>
+      </c>
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
       <c r="I31" s="15"/>
@@ -3081,8 +3131,12 @@
       </c>
       <c r="C32" s="28"/>
       <c r="D32" s="29"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
+      <c r="E32" s="14">
+        <v>19</v>
+      </c>
+      <c r="F32" s="14">
+        <v>14</v>
+      </c>
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
       <c r="I32" s="15"/>
@@ -3096,8 +3150,12 @@
       </c>
       <c r="C33" s="28"/>
       <c r="D33" s="29"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
+      <c r="E33" s="14">
+        <v>19</v>
+      </c>
+      <c r="F33" s="14">
+        <v>14</v>
+      </c>
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="15"/>

</xml_diff>

<commit_message>
finished functions for part 3.1
</commit_message>
<xml_diff>
--- a/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
+++ b/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A813B4-AD2C-4976-9F6F-5F2AB91378B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE300983-31DA-4748-BE3C-54887CB800C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2104,11 +2104,11 @@
   <dimension ref="A1:BO81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="AB10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="6" topLeftCell="AB20" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="AI16" sqref="AI16"/>
+      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2966,9 +2966,15 @@
       <c r="F23" s="14">
         <v>14</v>
       </c>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="15"/>
+      <c r="G23" s="14">
+        <v>19</v>
+      </c>
+      <c r="H23" s="14">
+        <v>1</v>
+      </c>
+      <c r="I23" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="47">

</xml_diff>

<commit_message>
add comments for fixing bugs in staff-class.cpp
</commit_message>
<xml_diff>
--- a/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
+++ b/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE300983-31DA-4748-BE3C-54887CB800C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB382E1B-4F7D-4ADC-8073-C9BB9B61AFFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2104,11 +2104,11 @@
   <dimension ref="A1:BO81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="AB20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="6" topLeftCell="AB40" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
+      <selection pane="bottomRight" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -3197,9 +3197,15 @@
       <c r="F35" s="14">
         <v>8</v>
       </c>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="15"/>
+      <c r="G35" s="14">
+        <v>15</v>
+      </c>
+      <c r="H35" s="14">
+        <v>5</v>
+      </c>
+      <c r="I35" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="47">
@@ -3210,12 +3216,8 @@
       </c>
       <c r="C36" s="28"/>
       <c r="D36" s="29"/>
-      <c r="E36" s="14">
-        <v>15</v>
-      </c>
-      <c r="F36" s="14">
-        <v>8</v>
-      </c>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
       <c r="I36" s="15"/>
@@ -3246,11 +3248,21 @@
       </c>
       <c r="C38" s="28"/>
       <c r="D38" s="29"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="15"/>
+      <c r="E38" s="14">
+        <v>15</v>
+      </c>
+      <c r="F38" s="14">
+        <v>8</v>
+      </c>
+      <c r="G38" s="14">
+        <v>15</v>
+      </c>
+      <c r="H38" s="14">
+        <v>5</v>
+      </c>
+      <c r="I38" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="47">
@@ -3419,7 +3431,7 @@
       <c r="H49" s="14"/>
       <c r="I49" s="15"/>
     </row>
-    <row r="50" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="47">
         <v>7.2</v>
       </c>

</xml_diff>

<commit_message>
update importClass and SearchScoreboard/Attendance functions
</commit_message>
<xml_diff>
--- a/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
+++ b/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB382E1B-4F7D-4ADC-8073-C9BB9B61AFFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F94D5F-710B-455D-AEC4-5D64D7D7FA51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2104,11 +2104,11 @@
   <dimension ref="A1:BO81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="AB40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="6" topLeftCell="AB10" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="D50" sqref="D50"/>
+      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2840,9 +2840,11 @@
       <c r="G15" s="14">
         <v>15</v>
       </c>
-      <c r="H15" s="14"/>
+      <c r="H15" s="14">
+        <v>10</v>
+      </c>
       <c r="I15" s="15">
-        <v>0.15</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="16" spans="1:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3216,11 +3218,21 @@
       </c>
       <c r="C36" s="28"/>
       <c r="D36" s="29"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="15"/>
+      <c r="E36" s="14">
+        <v>20</v>
+      </c>
+      <c r="F36" s="14">
+        <v>5</v>
+      </c>
+      <c r="G36" s="14">
+        <v>20</v>
+      </c>
+      <c r="H36" s="14">
+        <v>5</v>
+      </c>
+      <c r="I36" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="46">
@@ -3273,11 +3285,21 @@
       </c>
       <c r="C39" s="28"/>
       <c r="D39" s="29"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="15"/>
+      <c r="E39" s="14">
+        <v>20</v>
+      </c>
+      <c r="F39" s="14">
+        <v>5</v>
+      </c>
+      <c r="G39" s="14">
+        <v>20</v>
+      </c>
+      <c r="H39" s="14">
+        <v>5</v>
+      </c>
+      <c r="I39" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="46">

</xml_diff>

<commit_message>
addCourse function is halfway done
</commit_message>
<xml_diff>
--- a/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
+++ b/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F94D5F-710B-455D-AEC4-5D64D7D7FA51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D46A20-1367-4159-9275-84E7BD19DCBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2104,11 +2104,11 @@
   <dimension ref="A1:BO81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="AB10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="6" topLeftCell="AB20" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomRight" activeCell="AG26" sqref="AG26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -3025,12 +3025,8 @@
       </c>
       <c r="C26" s="28"/>
       <c r="D26" s="29"/>
-      <c r="E26" s="14">
-        <v>19</v>
-      </c>
-      <c r="F26" s="14">
-        <v>14</v>
-      </c>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
       <c r="I26" s="15"/>
@@ -3044,12 +3040,8 @@
       </c>
       <c r="C27" s="28"/>
       <c r="D27" s="29"/>
-      <c r="E27" s="14">
-        <v>19</v>
-      </c>
-      <c r="F27" s="14">
-        <v>14</v>
-      </c>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
       <c r="I27" s="15"/>
@@ -3063,12 +3055,8 @@
       </c>
       <c r="C28" s="28"/>
       <c r="D28" s="29"/>
-      <c r="E28" s="14">
-        <v>19</v>
-      </c>
-      <c r="F28" s="14">
-        <v>14</v>
-      </c>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
       <c r="I28" s="15"/>
@@ -3082,12 +3070,8 @@
       </c>
       <c r="C29" s="28"/>
       <c r="D29" s="29"/>
-      <c r="E29" s="14">
-        <v>19</v>
-      </c>
-      <c r="F29" s="14">
-        <v>14</v>
-      </c>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
       <c r="I29" s="15"/>
@@ -3101,12 +3085,8 @@
       </c>
       <c r="C30" s="28"/>
       <c r="D30" s="29"/>
-      <c r="E30" s="14">
-        <v>19</v>
-      </c>
-      <c r="F30" s="14">
-        <v>14</v>
-      </c>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
       <c r="I30" s="15"/>
@@ -3120,12 +3100,8 @@
       </c>
       <c r="C31" s="28"/>
       <c r="D31" s="29"/>
-      <c r="E31" s="14">
-        <v>19</v>
-      </c>
-      <c r="F31" s="14">
-        <v>14</v>
-      </c>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
       <c r="I31" s="15"/>
@@ -3139,12 +3115,8 @@
       </c>
       <c r="C32" s="28"/>
       <c r="D32" s="29"/>
-      <c r="E32" s="14">
-        <v>19</v>
-      </c>
-      <c r="F32" s="14">
-        <v>14</v>
-      </c>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
       <c r="I32" s="15"/>
@@ -3158,12 +3130,8 @@
       </c>
       <c r="C33" s="28"/>
       <c r="D33" s="29"/>
-      <c r="E33" s="14">
-        <v>19</v>
-      </c>
-      <c r="F33" s="14">
-        <v>14</v>
-      </c>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="15"/>
@@ -3615,7 +3583,7 @@
   </sheetPr>
   <dimension ref="A2:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="140" workbookViewId="0">
+    <sheetView zoomScale="140" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix some bugs in viewscore, viewcheckin, and importCourse functions
</commit_message>
<xml_diff>
--- a/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
+++ b/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B28F3DD-10F6-48E7-8040-0D7B0F17E146}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B69FD13-97EC-4304-B4DA-81C62C7D4BD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="135">
   <si>
     <t>Project Planner</t>
   </si>
@@ -1892,7 +1892,7 @@
   </sheetPr>
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -2103,12 +2103,12 @@
   </sheetPr>
   <dimension ref="A1:BO81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="Z7" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="10" ySplit="6" topLeftCell="K39" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="G44" sqref="G44"/>
+      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2901,8 +2901,12 @@
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="29"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
+      <c r="E19" s="14">
+        <v>32</v>
+      </c>
+      <c r="F19" s="14">
+        <v>4</v>
+      </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
       <c r="I19" s="15"/>
@@ -2916,8 +2920,12 @@
       </c>
       <c r="C20" s="28"/>
       <c r="D20" s="29"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
+      <c r="E20" s="14">
+        <v>32</v>
+      </c>
+      <c r="F20" s="14">
+        <v>4</v>
+      </c>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="15"/>
@@ -2931,8 +2939,12 @@
       </c>
       <c r="C21" s="28"/>
       <c r="D21" s="29"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="E21" s="14">
+        <v>32</v>
+      </c>
+      <c r="F21" s="14">
+        <v>4</v>
+      </c>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="15"/>
@@ -3037,8 +3049,12 @@
       </c>
       <c r="C26" s="28"/>
       <c r="D26" s="29"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
+      <c r="E26" s="14">
+        <v>32</v>
+      </c>
+      <c r="F26" s="14">
+        <v>7</v>
+      </c>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
       <c r="I26" s="15"/>
@@ -3052,8 +3068,12 @@
       </c>
       <c r="C27" s="28"/>
       <c r="D27" s="29"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
+      <c r="E27" s="14">
+        <v>32</v>
+      </c>
+      <c r="F27" s="14">
+        <v>7</v>
+      </c>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
       <c r="I27" s="15"/>
@@ -3141,9 +3161,15 @@
         <v>91</v>
       </c>
       <c r="C33" s="28"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
+      <c r="D33" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="E33" s="14">
+        <v>32</v>
+      </c>
+      <c r="F33" s="14">
+        <v>5</v>
+      </c>
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="15"/>
@@ -3444,11 +3470,21 @@
       <c r="D50" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="15"/>
+      <c r="E50" s="14">
+        <v>25</v>
+      </c>
+      <c r="F50" s="14">
+        <v>7</v>
+      </c>
+      <c r="G50" s="14">
+        <v>27</v>
+      </c>
+      <c r="H50" s="14">
+        <v>2</v>
+      </c>
+      <c r="I50" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="47">
@@ -3461,8 +3497,12 @@
       <c r="D51" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
+      <c r="E51" s="14">
+        <v>32</v>
+      </c>
+      <c r="F51" s="14">
+        <v>5</v>
+      </c>
       <c r="G51" s="14"/>
       <c r="H51" s="14"/>
       <c r="I51" s="15"/>
@@ -3478,11 +3518,21 @@
       <c r="D52" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="15"/>
+      <c r="E52" s="14">
+        <v>25</v>
+      </c>
+      <c r="F52" s="14">
+        <v>7</v>
+      </c>
+      <c r="G52" s="14">
+        <v>27</v>
+      </c>
+      <c r="H52" s="14">
+        <v>2</v>
+      </c>
+      <c r="I52" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="48"/>

</xml_diff>

<commit_message>
fixed addStudent, removeStudent, editStudent, viewClass function, added function to read Classes.txt
</commit_message>
<xml_diff>
--- a/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
+++ b/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C904094-7091-43A6-A212-19E08CE30235}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F56D64-41FA-419D-B379-D383AA2DA306}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="140">
   <si>
     <t>Project Planner</t>
   </si>
@@ -602,6 +602,21 @@
   </si>
   <si>
     <t>Import scoreboard of a course (midterm, final, bonus, total) from a csv file.</t>
+  </si>
+  <si>
+    <t>Group's Notes</t>
+  </si>
+  <si>
+    <t>Same as 6,2.</t>
+  </si>
+  <si>
+    <t>Same as 6,1.</t>
+  </si>
+  <si>
+    <t>Same as 6,3. Reuse codes from 5,1.</t>
+  </si>
+  <si>
+    <t>Reuse codes from 4,1.</t>
   </si>
 </sst>
 </file>
@@ -1063,7 +1078,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1249,17 +1264,23 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Đầu đề 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Siêu kết nối" xfId="8" builtinId="8"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -2104,16 +2125,16 @@
   <dimension ref="A1:BO81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="V10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="6" topLeftCell="K21" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
+      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6" style="45" customWidth="1"/>
+    <col min="1" max="1" width="7" style="45" customWidth="1"/>
     <col min="2" max="2" width="36.875" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.75" style="2" customWidth="1"/>
     <col min="4" max="4" width="20.25" style="2" customWidth="1"/>
@@ -3175,7 +3196,7 @@
       <c r="I31" s="15"/>
     </row>
     <row r="32" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="47">
+      <c r="A32" s="67">
         <v>3.1</v>
       </c>
       <c r="B32" s="58" t="s">
@@ -3681,8 +3702,8 @@
   </sheetPr>
   <dimension ref="A2:D23"/>
   <sheetViews>
-    <sheetView zoomScale="140" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A6" zoomScale="140" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3760,6 +3781,46 @@
       </c>
       <c r="C10" s="58" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="59"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3.8</v>
+      </c>
+      <c r="C13" s="58" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="59">
+        <v>3.9</v>
+      </c>
+      <c r="C14" s="58" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="68">
+        <v>3.1</v>
+      </c>
+      <c r="C15" s="58" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6.7</v>
+      </c>
+      <c r="C16" s="58" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
editCourse and removeCourse done!
</commit_message>
<xml_diff>
--- a/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
+++ b/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B6FDCA-667C-4D53-8FFA-C3BFC25F94CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="140">
   <si>
     <t>Project Planner</t>
   </si>
@@ -602,11 +603,26 @@
   <si>
     <t>Import scoreboard of a course (midterm, final, bonus, total) from a csv file.</t>
   </si>
+  <si>
+    <t>Group's Notes</t>
+  </si>
+  <si>
+    <t>Same as 6,2.</t>
+  </si>
+  <si>
+    <t>Same as 6,1.</t>
+  </si>
+  <si>
+    <t>Same as 6,3. Reuse codes from 5,1.</t>
+  </si>
+  <si>
+    <t>Reuse codes from 4,1.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="d/m"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
@@ -1062,7 +1078,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1242,6 +1258,12 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1250,15 +1272,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Activity" xfId="2"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8"/>
-    <cellStyle name="Label" xfId="5"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Percent Complete" xfId="6"/>
-    <cellStyle name="Period Headers" xfId="3"/>
-    <cellStyle name="Period Highlight Control" xfId="7"/>
-    <cellStyle name="Project Headers" xfId="4"/>
+    <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Đầu đề 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Siêu kết nối" xfId="8" builtinId="8"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -1451,16 +1473,19 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1029" name="Spinner 5" hidden="1">
+            <xdr:cNvPr id="1029" name="Spinner 5" descr="Period Highlight Spin Control" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1029"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1468,6 +1493,12 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData fPrintsWithSheet="0"/>
@@ -1479,13 +1510,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C6:F11" totalsRowShown="0">
-  <autoFilter ref="C6:F11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="C6:F11" totalsRowShown="0">
+  <autoFilter ref="C6:F11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="3" name="Email"/>
-    <tableColumn id="4" name="Slack username" dataDxfId="10"/>
-    <tableColumn id="2" name="Phone"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Email"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Slack username" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{0E6AA203-A562-47F1-A98F-70894F727552}" name="Phone"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1717,7 +1748,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
@@ -1737,36 +1768,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="65"/>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
+      <c r="A2" s="67"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="65"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
+      <c r="A3" s="67"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
     </row>
     <row r="6" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
@@ -1876,7 +1907,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
@@ -1896,33 +1927,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="65"/>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
+      <c r="A2" s="67"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
     </row>
     <row r="3" spans="1:7" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="65"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
+      <c r="A3" s="67"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
@@ -2073,9 +2104,9 @@
     <mergeCell ref="A1:G3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1"/>
-    <hyperlink ref="D7" r:id="rId2"/>
-    <hyperlink ref="D8" r:id="rId3"/>
+    <hyperlink ref="D9" r:id="rId1" xr:uid="{B1FC0B1B-B202-4FB4-849A-7217647E43C9}"/>
+    <hyperlink ref="D7" r:id="rId2" xr:uid="{1E5422A0-F933-4995-88B3-5E7171598377}"/>
+    <hyperlink ref="D8" r:id="rId3" xr:uid="{95866375-0D5E-45B3-84AE-4ECD81D7FF7B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
@@ -2086,7 +2117,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="1"/>
@@ -2094,16 +2125,16 @@
   <dimension ref="A1:BO81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="Z25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="6" topLeftCell="AE7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="D51" sqref="D51"/>
+      <selection pane="bottomRight" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6" style="45" customWidth="1"/>
+    <col min="1" max="1" width="7" style="45" customWidth="1"/>
     <col min="2" max="2" width="36.875" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.75" style="2" customWidth="1"/>
     <col min="4" max="4" width="20.25" style="2" customWidth="1"/>
@@ -2138,26 +2169,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:67" ht="15" x14ac:dyDescent="0.25">
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
     </row>
     <row r="2" spans="1:67" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
       <c r="K2" s="7" t="s">
         <v>14</v>
       </c>
@@ -2195,14 +2226,14 @@
       </c>
     </row>
     <row r="3" spans="1:67" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
       <c r="AV3" s="1"/>
       <c r="AW3" s="1"/>
       <c r="AX3" s="1"/>
@@ -2846,11 +2877,21 @@
       </c>
       <c r="C16" s="28"/>
       <c r="D16" s="29"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="15"/>
+      <c r="E16" s="14">
+        <v>25</v>
+      </c>
+      <c r="F16" s="14">
+        <v>10</v>
+      </c>
+      <c r="G16" s="14">
+        <v>25</v>
+      </c>
+      <c r="H16" s="14">
+        <v>10</v>
+      </c>
+      <c r="I16" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="47">
@@ -2861,11 +2902,21 @@
       </c>
       <c r="C17" s="28"/>
       <c r="D17" s="29"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="15"/>
+      <c r="E17" s="14">
+        <v>25</v>
+      </c>
+      <c r="F17" s="14">
+        <v>10</v>
+      </c>
+      <c r="G17" s="14">
+        <v>25</v>
+      </c>
+      <c r="H17" s="14">
+        <v>10</v>
+      </c>
+      <c r="I17" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="47">
@@ -2876,11 +2927,21 @@
       </c>
       <c r="C18" s="28"/>
       <c r="D18" s="29"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="15"/>
+      <c r="E18" s="14">
+        <v>30</v>
+      </c>
+      <c r="F18" s="14">
+        <v>10</v>
+      </c>
+      <c r="G18" s="14">
+        <v>30</v>
+      </c>
+      <c r="H18" s="14">
+        <v>10</v>
+      </c>
+      <c r="I18" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="47">
@@ -2891,11 +2952,21 @@
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="29"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="15"/>
+      <c r="E19" s="14">
+        <v>32</v>
+      </c>
+      <c r="F19" s="14">
+        <v>10</v>
+      </c>
+      <c r="G19" s="14">
+        <v>32</v>
+      </c>
+      <c r="H19" s="14">
+        <v>0</v>
+      </c>
+      <c r="I19" s="15">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="47">
@@ -2906,11 +2977,21 @@
       </c>
       <c r="C20" s="28"/>
       <c r="D20" s="29"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="15"/>
+      <c r="E20" s="14">
+        <v>32</v>
+      </c>
+      <c r="F20" s="14">
+        <v>10</v>
+      </c>
+      <c r="G20" s="14">
+        <v>32</v>
+      </c>
+      <c r="H20" s="14">
+        <v>10</v>
+      </c>
+      <c r="I20" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="47">
@@ -2921,11 +3002,21 @@
       </c>
       <c r="C21" s="28"/>
       <c r="D21" s="29"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="15"/>
+      <c r="E21" s="14">
+        <v>32</v>
+      </c>
+      <c r="F21" s="14">
+        <v>10</v>
+      </c>
+      <c r="G21" s="14">
+        <v>32</v>
+      </c>
+      <c r="H21" s="14">
+        <v>10</v>
+      </c>
+      <c r="I21" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="46">
@@ -3027,11 +3118,21 @@
       </c>
       <c r="C26" s="28"/>
       <c r="D26" s="29"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="15"/>
+      <c r="E26" s="14">
+        <v>32</v>
+      </c>
+      <c r="F26" s="14">
+        <v>7</v>
+      </c>
+      <c r="G26" s="14">
+        <v>32</v>
+      </c>
+      <c r="H26" s="14">
+        <v>7</v>
+      </c>
+      <c r="I26" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="47">
@@ -3042,11 +3143,21 @@
       </c>
       <c r="C27" s="28"/>
       <c r="D27" s="29"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="15"/>
+      <c r="E27" s="14">
+        <v>32</v>
+      </c>
+      <c r="F27" s="14">
+        <v>7</v>
+      </c>
+      <c r="G27" s="14">
+        <v>32</v>
+      </c>
+      <c r="H27" s="14">
+        <v>7</v>
+      </c>
+      <c r="I27" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="47">
@@ -3109,7 +3220,7 @@
       <c r="I31" s="15"/>
     </row>
     <row r="32" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="47">
+      <c r="A32" s="65">
         <v>3.1</v>
       </c>
       <c r="B32" s="58" t="s">
@@ -3131,12 +3242,24 @@
         <v>91</v>
       </c>
       <c r="C33" s="28"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="15"/>
+      <c r="D33" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="E33" s="14">
+        <v>41</v>
+      </c>
+      <c r="F33" s="14">
+        <v>2</v>
+      </c>
+      <c r="G33" s="14">
+        <v>41</v>
+      </c>
+      <c r="H33" s="14">
+        <v>2</v>
+      </c>
+      <c r="I33" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="46">
@@ -3434,11 +3557,21 @@
       <c r="D50" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="15"/>
+      <c r="E50" s="14">
+        <v>25</v>
+      </c>
+      <c r="F50" s="14">
+        <v>7</v>
+      </c>
+      <c r="G50" s="14">
+        <v>27</v>
+      </c>
+      <c r="H50" s="14">
+        <v>2</v>
+      </c>
+      <c r="I50" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="47">
@@ -3451,11 +3584,21 @@
       <c r="D51" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="15"/>
+      <c r="E51" s="14">
+        <v>41</v>
+      </c>
+      <c r="F51" s="14">
+        <v>2</v>
+      </c>
+      <c r="G51" s="14">
+        <v>41</v>
+      </c>
+      <c r="H51" s="14">
+        <v>2</v>
+      </c>
+      <c r="I51" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="52" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="47">
@@ -3468,11 +3611,21 @@
       <c r="D52" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="15"/>
+      <c r="E52" s="14">
+        <v>25</v>
+      </c>
+      <c r="F52" s="14">
+        <v>7</v>
+      </c>
+      <c r="G52" s="14">
+        <v>27</v>
+      </c>
+      <c r="H52" s="14">
+        <v>2</v>
+      </c>
+      <c r="I52" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="48"/>
@@ -3579,14 +3732,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{167154E8-4B3C-4AE3-A2D5-CEB0BD01F89A}">
   <sheetPr>
     <tabColor theme="6" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A2:D23"/>
   <sheetViews>
-    <sheetView zoomScale="140" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A6" zoomScale="140" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3664,6 +3817,46 @@
       </c>
       <c r="C10" s="58" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="59"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3.8</v>
+      </c>
+      <c r="C13" s="58" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="59">
+        <v>3.9</v>
+      </c>
+      <c r="C14" s="58" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="66">
+        <v>3.1</v>
+      </c>
+      <c r="C15" s="58" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6.7</v>
+      </c>
+      <c r="C16" s="58" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
addCourseStudent and removeCourseStudent done!
Also implemented in the main program
</commit_message>
<xml_diff>
--- a/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
+++ b/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C29AB0-3686-41A9-A79C-2AB907C03EDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6768299-E6AD-4F36-B245-E183DEE6B6EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2125,11 +2125,11 @@
   <dimension ref="A1:BO81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="K40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="6" topLeftCell="R40" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="G48" sqref="G48"/>
+      <selection pane="bottomRight" activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -3174,9 +3174,15 @@
       <c r="F28" s="14">
         <v>11</v>
       </c>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="15"/>
+      <c r="G28" s="14">
+        <v>40</v>
+      </c>
+      <c r="H28" s="14">
+        <v>7</v>
+      </c>
+      <c r="I28" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="47">
@@ -3193,9 +3199,15 @@
       <c r="F29" s="14">
         <v>11</v>
       </c>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="15"/>
+      <c r="G29" s="14">
+        <v>40</v>
+      </c>
+      <c r="H29" s="14">
+        <v>7</v>
+      </c>
+      <c r="I29" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="47">

</xml_diff>

<commit_message>
student checkin function done
</commit_message>
<xml_diff>
--- a/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
+++ b/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6768299-E6AD-4F36-B245-E183DEE6B6EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE134F8-938B-40E4-9375-E2766D4495B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="141">
   <si>
     <t>Project Planner</t>
   </si>
@@ -617,6 +617,9 @@
   </si>
   <si>
     <t>Reuse codes from 4,1.</t>
+  </si>
+  <si>
+    <t>(Function Removed)</t>
   </si>
 </sst>
 </file>
@@ -2125,11 +2128,11 @@
   <dimension ref="A1:BO81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="R40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="6" topLeftCell="N48" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="T19" sqref="T19"/>
+      <selection pane="bottomRight" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -3224,7 +3227,7 @@
         <v>40</v>
       </c>
       <c r="F30" s="14">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
@@ -3245,7 +3248,7 @@
         <v>40</v>
       </c>
       <c r="F31" s="14">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
@@ -3259,7 +3262,9 @@
         <v>90</v>
       </c>
       <c r="C32" s="28"/>
-      <c r="D32" s="29"/>
+      <c r="D32" s="29" t="s">
+        <v>140</v>
+      </c>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
@@ -3502,7 +3507,7 @@
         <v>40</v>
       </c>
       <c r="F44" s="14">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G44" s="14"/>
       <c r="H44" s="14"/>
@@ -3523,7 +3528,7 @@
         <v>40</v>
       </c>
       <c r="F45" s="14">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G45" s="14"/>
       <c r="H45" s="14"/>
@@ -3544,7 +3549,7 @@
         <v>40</v>
       </c>
       <c r="F46" s="14">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G46" s="14"/>
       <c r="H46" s="14"/>
@@ -3596,9 +3601,15 @@
       <c r="F49" s="14">
         <v>11</v>
       </c>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="15"/>
+      <c r="G49" s="14">
+        <v>40</v>
+      </c>
+      <c r="H49" s="14">
+        <v>11</v>
+      </c>
+      <c r="I49" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="47">

</xml_diff>

<commit_message>
add sortAccount and sortStudent functions
Also implemented them in addCourseStudent, importClass, addStudent functions
</commit_message>
<xml_diff>
--- a/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
+++ b/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE134F8-938B-40E4-9375-E2766D4495B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4035E395-E5C7-4B6F-930C-5491B92BA5FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2128,11 +2128,11 @@
   <dimension ref="A1:BO81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="N48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="6" topLeftCell="K22" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="F35" sqref="F35"/>
+      <selection pane="bottomRight" activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -3602,10 +3602,10 @@
         <v>11</v>
       </c>
       <c r="G49" s="14">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="H49" s="14">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="I49" s="15">
         <v>1</v>

</xml_diff>

<commit_message>
fix some bugs in display functions
</commit_message>
<xml_diff>
--- a/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
+++ b/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4035E395-E5C7-4B6F-930C-5491B92BA5FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1E1EBC-4309-4120-8299-8872E17D32CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2128,11 +2128,11 @@
   <dimension ref="A1:BO81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="K22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="6" topLeftCell="K39" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="H49" sqref="H49"/>
+      <selection pane="bottomRight" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update the group's plan
</commit_message>
<xml_diff>
--- a/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
+++ b/KTLT_19CLC5_Group11_FinalProjectPlan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1E1EBC-4309-4120-8299-8872E17D32CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118D7D69-8ED1-4655-AA18-7C6201115908}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="141">
   <si>
     <t>Project Planner</t>
   </si>
@@ -2128,11 +2128,11 @@
   <dimension ref="A1:BO81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="K39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="6" topLeftCell="AC39" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="B42" sqref="B42"/>
+      <selection pane="bottomRight" activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2965,10 +2965,10 @@
         <v>32</v>
       </c>
       <c r="H19" s="14">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I19" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3028,9 +3028,7 @@
       <c r="B22" s="60" t="s">
         <v>123</v>
       </c>
-      <c r="D22" s="42" t="s">
-        <v>120</v>
-      </c>
+      <c r="D22" s="42"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
@@ -3045,7 +3043,9 @@
         <v>80</v>
       </c>
       <c r="C23" s="28"/>
-      <c r="D23" s="29"/>
+      <c r="D23" s="29" t="s">
+        <v>120</v>
+      </c>
       <c r="E23" s="14">
         <v>19</v>
       </c>
@@ -3070,7 +3070,9 @@
         <v>114</v>
       </c>
       <c r="C24" s="28"/>
-      <c r="D24" s="29"/>
+      <c r="D24" s="29" t="s">
+        <v>120</v>
+      </c>
       <c r="E24" s="14">
         <v>19</v>
       </c>
@@ -3095,7 +3097,9 @@
         <v>83</v>
       </c>
       <c r="C25" s="28"/>
-      <c r="D25" s="29"/>
+      <c r="D25" s="29" t="s">
+        <v>120</v>
+      </c>
       <c r="E25" s="14">
         <v>19</v>
       </c>
@@ -3120,7 +3124,9 @@
         <v>84</v>
       </c>
       <c r="C26" s="28"/>
-      <c r="D26" s="29"/>
+      <c r="D26" s="29" t="s">
+        <v>120</v>
+      </c>
       <c r="E26" s="14">
         <v>32</v>
       </c>
@@ -3145,7 +3151,9 @@
         <v>85</v>
       </c>
       <c r="C27" s="28"/>
-      <c r="D27" s="29"/>
+      <c r="D27" s="29" t="s">
+        <v>120</v>
+      </c>
       <c r="E27" s="14">
         <v>32</v>
       </c>
@@ -3170,7 +3178,9 @@
         <v>115</v>
       </c>
       <c r="C28" s="28"/>
-      <c r="D28" s="29"/>
+      <c r="D28" s="29" t="s">
+        <v>120</v>
+      </c>
       <c r="E28" s="14">
         <v>40</v>
       </c>
@@ -3195,7 +3205,9 @@
         <v>116</v>
       </c>
       <c r="C29" s="28"/>
-      <c r="D29" s="29"/>
+      <c r="D29" s="29" t="s">
+        <v>120</v>
+      </c>
       <c r="E29" s="14">
         <v>40</v>
       </c>
@@ -3229,9 +3241,15 @@
       <c r="F30" s="14">
         <v>14</v>
       </c>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="15"/>
+      <c r="G30" s="14">
+        <v>40</v>
+      </c>
+      <c r="H30" s="14">
+        <v>14</v>
+      </c>
+      <c r="I30" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="47">
@@ -3250,9 +3268,15 @@
       <c r="F31" s="14">
         <v>14</v>
       </c>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="15"/>
+      <c r="G31" s="14">
+        <v>40</v>
+      </c>
+      <c r="H31" s="14">
+        <v>14</v>
+      </c>
+      <c r="I31" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="65">
@@ -3438,9 +3462,7 @@
       <c r="B40" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="D40" s="42" t="s">
-        <v>122</v>
-      </c>
+      <c r="D40" s="42"/>
       <c r="E40" s="14"/>
       <c r="F40" s="14"/>
       <c r="G40" s="14"/>
@@ -3455,12 +3477,24 @@
         <v>88</v>
       </c>
       <c r="C41" s="28"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="15"/>
+      <c r="D41" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="E41" s="14">
+        <v>40</v>
+      </c>
+      <c r="F41" s="14">
+        <v>14</v>
+      </c>
+      <c r="G41" s="14">
+        <v>40</v>
+      </c>
+      <c r="H41" s="14">
+        <v>14</v>
+      </c>
+      <c r="I41" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="47">
@@ -3470,12 +3504,24 @@
         <v>89</v>
       </c>
       <c r="C42" s="28"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="15"/>
+      <c r="D42" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="E42" s="14">
+        <v>40</v>
+      </c>
+      <c r="F42" s="14">
+        <v>14</v>
+      </c>
+      <c r="G42" s="14">
+        <v>40</v>
+      </c>
+      <c r="H42" s="14">
+        <v>14</v>
+      </c>
+      <c r="I42" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="47">
@@ -3485,12 +3531,24 @@
         <v>90</v>
       </c>
       <c r="C43" s="28"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="15"/>
+      <c r="D43" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="E43" s="14">
+        <v>15</v>
+      </c>
+      <c r="F43" s="14">
+        <v>8</v>
+      </c>
+      <c r="G43" s="14">
+        <v>15</v>
+      </c>
+      <c r="H43" s="14">
+        <v>5</v>
+      </c>
+      <c r="I43" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="47">
@@ -3509,9 +3567,13 @@
       <c r="F44" s="14">
         <v>14</v>
       </c>
-      <c r="G44" s="14"/>
+      <c r="G44" s="14">
+        <v>40</v>
+      </c>
       <c r="H44" s="14"/>
-      <c r="I44" s="15"/>
+      <c r="I44" s="15">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="47">
@@ -3530,9 +3592,13 @@
       <c r="F45" s="14">
         <v>14</v>
       </c>
-      <c r="G45" s="14"/>
+      <c r="G45" s="14">
+        <v>40</v>
+      </c>
       <c r="H45" s="14"/>
-      <c r="I45" s="15"/>
+      <c r="I45" s="15">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="47">
@@ -3551,9 +3617,13 @@
       <c r="F46" s="14">
         <v>14</v>
       </c>
-      <c r="G46" s="14"/>
+      <c r="G46" s="14">
+        <v>40</v>
+      </c>
       <c r="H46" s="14"/>
-      <c r="I46" s="15"/>
+      <c r="I46" s="15">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="47">
@@ -3563,12 +3633,24 @@
         <v>98</v>
       </c>
       <c r="C47" s="28"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="15"/>
+      <c r="D47" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="E47" s="14">
+        <v>15</v>
+      </c>
+      <c r="F47" s="14">
+        <v>8</v>
+      </c>
+      <c r="G47" s="14">
+        <v>15</v>
+      </c>
+      <c r="H47" s="14">
+        <v>5</v>
+      </c>
+      <c r="I47" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="46">

</xml_diff>